<commit_message>
evidencia ns semana 20
</commit_message>
<xml_diff>
--- a/semana/semana_completa_20.xlsx
+++ b/semana/semana_completa_20.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28922"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE341774-3ACF-4975-A6C6-E54C4A54744A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AF4A39B-6780-4C78-A450-3C55426BEE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3577" uniqueCount="637">
   <si>
     <t>c</t>
   </si>
@@ -1696,13 +1696,268 @@
   </si>
   <si>
     <t>Observacion</t>
+  </si>
+  <si>
+    <t>Puntual</t>
+  </si>
+  <si>
+    <t>No registra el tiempo de llegada real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega en tiempo </t>
+  </si>
+  <si>
+    <t>5 a 10 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No registra hora real </t>
+  </si>
+  <si>
+    <t>Inicia en tiempo</t>
+  </si>
+  <si>
+    <t>11 a 15 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un viaje inicia tarde y no registra punto 1 la hora real </t>
+  </si>
+  <si>
+    <t xml:space="preserve">un viaje inicia tarde y no registra punto 1 la hora real,1 viaje llego 40 minutos tarde </t>
+  </si>
+  <si>
+    <t>mayor a 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia 35 minutos y otro inicia 26 miutnos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega 36 minutos tarde </t>
+  </si>
+  <si>
+    <t>1 viaje inicia 30 min tarde , 1 viaje llega 22 min tarde y 1 viaje no registra llegada real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 viajes incian mas de 25 min tarde y 2 puntual , 2 viajes llegan mas de 25 min tarde y 2 viajes llegan 11 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicia 50 min tarde, llega 40 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega a 26 a 30 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se desvia y llega 34 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 viajes incian puntual y 2 viajes inician mas de 20 min, llegan 3 viajes de 5 a 11 min tarde,y 4 viajes de 20 a 50 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viajes llega 40 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 30 min tarde y llega 40 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 3 viajes de 17 a 40 min tarde , 3 viajes llegan 33 a 53 min tarde y 2 viajes 8 mintas tarde </t>
+  </si>
+  <si>
+    <t>16 a 20 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cambiaron el horario, por trafico llegan 25 a 50 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia puntual y llega 9 min tarde a planta , el segun viaje incia tarde y llega 23 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje es unidad incorrecta </t>
+  </si>
+  <si>
+    <t>inicia 58 min tarde  y llega 22 min tarde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia 16 min y otro a 27 min tarde, 5 viajes llegan 21 a 39 min tarde y 1 viaje llega 6 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 48 min tarde  y llega 31 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia 5 min tarde y otro 24 min tarde , </t>
+  </si>
+  <si>
+    <t>No empieza en p 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia en punto 2 y llega temprano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">realiza otro recorrido y al finalizarlo incia el recorrido programado he inicia tarde, llega tarde 48 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llegan temprano a planta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viajes inicia puntual y 1 viaje inicia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega 3 minutos tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia punto 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llegaron a tiempo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 viajes no registro la llega real y llegan en tiempo , 2 viajes si llegan tarde 21 min y 6 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia punto 2 y tarde , </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llegan 2 viajes a 11 min tarde y 2 viajes 23 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje llego temprano y no registro la llegada real </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viajes fue unidad incorrecta </t>
+  </si>
+  <si>
+    <t>un viaje inicia punto 2 y realiza otra paradas por cual el atraso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia tarde por trafico a punto 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 viajes llegan a planta mas de 20 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">error de sistema no registra hora real de llegada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 viajes inician 5 a 10 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 39 min tarde y llega 29 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 40 min tarde </t>
+  </si>
+  <si>
+    <t>inicia punto 2 y tarde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 viajes llegan a planta 11 min tarde y 2 llegan mas de 30 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">un viaje llega a 20 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje llega 28 min tarde y otro viaje llega 8 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia 5 min tarde, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia 19 min tarde, 1 viaje llega 27 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia a mediados  y llega temprano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega 31 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">unidad incorrecta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">un viaje inicia 39 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inician 24 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicio unidad de traslada muy lejos para iniciar recorrido,3 viajes llegan de 24 a 50 min tarde y 1 viajes llega 8 mintos tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 54 min tarde, llega 36 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia y se va a valle del roble he inicia tarde 34 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 26 min, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia en tiempo, 1 solo viaje llega 56 min ya que se desvia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 32 min tarde por realizar otro recorrido </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 viajes inician en tiempo y no lo registra, 1 viaje llega 38 min tarde y 1 viaje llega 5 min tarde  </t>
+  </si>
+  <si>
+    <t>inicio 3 minutos tarde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viajes llega 27 min y otro viaje llega 5 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 viajes llegan 20 min tarde y 2 viajes llegan 11 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viajes llega 28 min tarde y otro viaje 5 min tarde  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia 24 min tarde, 3 viajes llegan 5 a 10 min y 1 viaje llega 28 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 viajes llegan  5 a 13 min tarde y 2 viajes llegan 20 a 35 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">en los recorridos inicia en punto 2, 2 viajes llegan 15 a 18 min tarde y 2 viajes mas de 20 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje no registra la hora real, algunos viajes no registro la hora real de llega pero igual llegaba tarde a planta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 viaje inicia 38 min , 3 viajes llegan mas de 21 min tarde a planta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no registra el horario real de inicio , solo 2 viajes llegan de 37 a 52 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega 36 min tarde se desvia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega 32 min tarde  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega 30 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 42 min tarde, llega 40 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llega 39 min tarde </t>
+  </si>
+  <si>
+    <t xml:space="preserve">un viaje inicia puntual, 1 viaje llega 17 min y otro en 7 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inicia 33 min tarde, y llega a planta 41 min </t>
+  </si>
+  <si>
+    <t>llega 36 min tarde</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1763,19 +2018,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1789,7 +2031,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1922,56 +2164,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF63BE7B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE082"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFED480"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDBC7B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFEC87E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB9975"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA8D72"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8696B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2018,21 +2212,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF46B1E1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2083,19 +2268,11 @@
     <xf numFmtId="0" fontId="8" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -31563,7 +31740,7 @@
       <c r="D496">
         <v>5</v>
       </c>
-      <c r="E496" s="47">
+      <c r="E496" s="36">
         <v>1</v>
       </c>
       <c r="F496" s="31">
@@ -31584,7 +31761,7 @@
       <c r="D497">
         <v>5</v>
       </c>
-      <c r="E497" s="47">
+      <c r="E497" s="36">
         <v>1</v>
       </c>
       <c r="F497" s="31">
@@ -33944,508 +34121,508 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="48">
+      <c r="B2" s="37">
         <v>22</v>
       </c>
-      <c r="C2" s="48">
+      <c r="C2" s="37">
         <v>0.91062142733569595</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="37">
         <v>5</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="37">
         <v>0.955268241420415</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="37">
         <v>3</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="37">
         <v>0.98345755693581804</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="37">
         <v>4</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="37">
         <v>0.95649304713396399</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="48">
-        <v>1</v>
-      </c>
-      <c r="C6" s="48">
+      <c r="B6" s="37">
+        <v>1</v>
+      </c>
+      <c r="C6" s="37">
         <v>0.88548387096774195</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="48">
+      <c r="B7" s="37">
         <v>15</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="37">
         <v>0.827900103009791</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="48">
-        <v>1</v>
-      </c>
-      <c r="C8" s="48">
+      <c r="B8" s="37">
+        <v>1</v>
+      </c>
+      <c r="C8" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="48">
+      <c r="B9" s="37">
         <v>14</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="37">
         <v>0.79233260781762804</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="37">
         <v>26</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="37">
         <v>0.89737704225590897</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="37">
         <v>4</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C11" s="37">
         <v>0.72685185185185197</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="37">
         <v>6</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="37">
         <v>0.95197901959588604</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="48">
+      <c r="B13" s="37">
         <v>7</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="37">
         <v>3</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="37">
         <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="37">
         <v>5</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="37">
         <v>0.93053224849563498</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="37">
         <v>7</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="37">
         <v>0.97146061218463897</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="48">
+      <c r="B17" s="37">
         <v>10</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="37">
         <v>0.91528790141296101</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="37">
         <v>9</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="37">
         <v>0.98228899388319701</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="48">
-        <v>1</v>
-      </c>
-      <c r="C19" s="48">
+      <c r="B19" s="37">
+        <v>1</v>
+      </c>
+      <c r="C19" s="37">
         <v>0.92857142857142905</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="48">
+      <c r="B20" s="37">
         <v>11</v>
       </c>
-      <c r="C20" s="48">
+      <c r="C20" s="37">
         <v>0.86581370161351601</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="48">
+      <c r="B21" s="37">
         <v>7</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="37">
         <v>0.93197278911564596</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="37">
         <v>3</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="37">
         <v>0.96028892733333104</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="48">
-        <v>1</v>
-      </c>
-      <c r="C23" s="48">
+      <c r="B23" s="37">
+        <v>1</v>
+      </c>
+      <c r="C23" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="48">
+      <c r="B24" s="37">
         <v>28</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="37">
         <v>0.83801539146245196</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="48">
+      <c r="B25" s="37">
         <v>4</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="37">
         <v>0.75</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="48">
-        <v>1</v>
-      </c>
-      <c r="C26" s="48">
+      <c r="B26" s="37">
+        <v>1</v>
+      </c>
+      <c r="C26" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="48">
+      <c r="B27" s="37">
         <v>5</v>
       </c>
-      <c r="C27" s="48">
+      <c r="C27" s="37">
         <v>0.95558608058608097</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="37">
         <v>13</v>
       </c>
-      <c r="C28" s="48">
+      <c r="C28" s="37">
         <v>0.81320884629155299</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="48">
+      <c r="B29" s="37">
         <v>8</v>
       </c>
-      <c r="C29" s="48">
+      <c r="C29" s="37">
         <v>0.96384847420498398</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="48">
-        <v>1</v>
-      </c>
-      <c r="C30" s="48">
+      <c r="B30" s="37">
+        <v>1</v>
+      </c>
+      <c r="C30" s="37">
         <v>0.84114583333333304</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="48">
+      <c r="B31" s="37">
         <v>6</v>
       </c>
-      <c r="C31" s="48">
+      <c r="C31" s="37">
         <v>0.97662037037036997</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="48">
+      <c r="B32" s="37">
         <v>7</v>
       </c>
-      <c r="C32" s="48">
+      <c r="C32" s="37">
         <v>0.98117118413992199</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="48">
-        <v>1</v>
-      </c>
-      <c r="C33" s="48">
+      <c r="B33" s="37">
+        <v>1</v>
+      </c>
+      <c r="C33" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="48">
+      <c r="B34" s="37">
         <v>5</v>
       </c>
-      <c r="C34" s="48">
+      <c r="C34" s="37">
         <v>0.865151515151515</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="48">
-        <v>1</v>
-      </c>
-      <c r="C35" s="48">
+      <c r="B35" s="37">
+        <v>1</v>
+      </c>
+      <c r="C35" s="37">
         <v>0.91428571428571404</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="48">
+      <c r="B36" s="37">
         <v>6</v>
       </c>
-      <c r="C36" s="48">
+      <c r="C36" s="37">
         <v>0.99663299663299698</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="48">
+      <c r="B37" s="37">
         <v>7</v>
       </c>
-      <c r="C37" s="48">
+      <c r="C37" s="37">
         <v>0.83285849693412695</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="48">
-        <v>1</v>
-      </c>
-      <c r="C38" s="48">
+      <c r="B38" s="37">
+        <v>1</v>
+      </c>
+      <c r="C38" s="37">
         <v>0.83838383838383801</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="48">
+      <c r="B39" s="37">
         <v>76</v>
       </c>
-      <c r="C39" s="48">
+      <c r="C39" s="37">
         <v>0.89186575057528095</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="48">
+      <c r="B40" s="37">
         <v>2</v>
       </c>
-      <c r="C40" s="48">
+      <c r="C40" s="37">
         <v>0.99583333333333302</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="48" t="s">
+      <c r="A41" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="48">
+      <c r="B41" s="37">
         <v>10</v>
       </c>
-      <c r="C41" s="48">
+      <c r="C41" s="37">
         <v>0.78333333333333299</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="48">
+      <c r="B42" s="37">
         <v>9</v>
       </c>
-      <c r="C42" s="48">
+      <c r="C42" s="37">
         <v>0.77477544746063298</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="48">
+      <c r="B43" s="37">
         <v>3</v>
       </c>
-      <c r="C43" s="48">
+      <c r="C43" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="48" t="s">
+      <c r="A44" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="48">
+      <c r="B44" s="37">
         <v>15</v>
       </c>
-      <c r="C44" s="48">
+      <c r="C44" s="37">
         <v>0.69825271035327596</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="48" t="s">
+      <c r="A45" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="48">
+      <c r="B45" s="37">
         <v>4</v>
       </c>
-      <c r="C45" s="48">
+      <c r="C45" s="37">
         <v>0.98750000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="48" t="s">
+      <c r="A46" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="48">
-        <v>1</v>
-      </c>
-      <c r="C46" s="48">
+      <c r="B46" s="37">
+        <v>1</v>
+      </c>
+      <c r="C46" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="48" t="s">
+      <c r="A47" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="48">
+      <c r="B47" s="37">
         <v>46</v>
       </c>
-      <c r="C47" s="48">
+      <c r="C47" s="37">
         <v>0.91604103826929895</v>
       </c>
     </row>
@@ -34503,7 +34680,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123B88C3-7251-47CF-A744-0BF7EF379447}">
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F90" sqref="F90"/>
@@ -34535,870 +34712,2589 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="36"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="36"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="38"/>
+      <c r="A3" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>552</v>
+      </c>
+      <c r="E3" t="s">
+        <v>553</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="36"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="A4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>552</v>
+      </c>
+      <c r="E4" t="s">
+        <v>555</v>
+      </c>
       <c r="F4" s="38"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="36"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="38"/>
+      <c r="A5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>556</v>
+      </c>
+      <c r="E5" t="s">
+        <v>555</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="36"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="A6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>552</v>
+      </c>
+      <c r="E6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="36"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
+      <c r="A7" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>556</v>
+      </c>
+      <c r="E7" t="s">
+        <v>558</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="36"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="A8" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>552</v>
+      </c>
+      <c r="E8" t="s">
+        <v>555</v>
+      </c>
       <c r="F8" s="38"/>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="36"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
+    <row r="9" spans="1:6" ht="30.75">
+      <c r="A9" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>558</v>
+      </c>
+      <c r="E9" t="s">
+        <v>555</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="41"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="A10" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>561</v>
+      </c>
+      <c r="E10" t="s">
+        <v>558</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="36"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
+      <c r="A11" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>552</v>
+      </c>
+      <c r="E11" t="s">
+        <v>555</v>
+      </c>
       <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="36"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="A12" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>555</v>
+      </c>
+      <c r="E12" t="s">
+        <v>558</v>
+      </c>
       <c r="F12" s="38"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="36"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
+      <c r="A13" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>555</v>
+      </c>
+      <c r="E13" t="s">
+        <v>561</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="36"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
+      <c r="A14" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>555</v>
+      </c>
+      <c r="E14" t="s">
+        <v>558</v>
+      </c>
       <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="36"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="36"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="38"/>
+      <c r="A15" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>552</v>
+      </c>
+      <c r="E15" t="s">
+        <v>555</v>
+      </c>
+      <c r="F15" s="38"/>
+    </row>
+    <row r="16" spans="1:6" ht="30.75">
+      <c r="A16" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>561</v>
+      </c>
+      <c r="E16" t="s">
+        <v>561</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="36"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="38"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="36"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="A17" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>555</v>
+      </c>
+      <c r="E17" t="s">
+        <v>553</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30.75">
+      <c r="A18" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>561</v>
+      </c>
+      <c r="E18" t="s">
+        <v>561</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="36"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
+      <c r="A19" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>561</v>
+      </c>
+      <c r="E19" t="s">
+        <v>561</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="36"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
+      <c r="A20" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>552</v>
+      </c>
+      <c r="E20" t="s">
+        <v>561</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="36"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
+      <c r="A21" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>552</v>
+      </c>
+      <c r="E21" t="s">
+        <v>561</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="36"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
+      <c r="A22" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>552</v>
+      </c>
+      <c r="E22" t="s">
+        <v>555</v>
+      </c>
       <c r="F22" s="38"/>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="36"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
+    <row r="23" spans="1:6" ht="30.75">
+      <c r="A23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>552</v>
+      </c>
+      <c r="E23" t="s">
+        <v>561</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="36"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="38"/>
+      <c r="A24" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>555</v>
+      </c>
+      <c r="E24" t="s">
+        <v>555</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="36"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="36"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="38"/>
+      <c r="A25" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>561</v>
+      </c>
+      <c r="E25" t="s">
+        <v>561</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30.75">
+      <c r="A26" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>561</v>
+      </c>
+      <c r="E26" t="s">
+        <v>561</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="36"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
+      <c r="A27" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>573</v>
+      </c>
+      <c r="E27" t="s">
+        <v>558</v>
+      </c>
       <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="36"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
+      <c r="A28" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>555</v>
+      </c>
+      <c r="E28" t="s">
+        <v>555</v>
+      </c>
       <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="36"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="41"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="38"/>
+      <c r="A29" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>558</v>
+      </c>
+      <c r="E29" t="s">
+        <v>561</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30.75">
+      <c r="A30" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>558</v>
+      </c>
+      <c r="E30" t="s">
+        <v>561</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="36"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
+      <c r="A31" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>573</v>
+      </c>
+      <c r="E31" t="s">
+        <v>555</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="36"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
+      <c r="A32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>552</v>
+      </c>
+      <c r="E32" t="s">
+        <v>555</v>
+      </c>
+      <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="41"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
+      <c r="A33" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>558</v>
+      </c>
+      <c r="E33" t="s">
+        <v>555</v>
+      </c>
+      <c r="F33" s="38"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="41"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="38"/>
+      <c r="A34" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>561</v>
+      </c>
+      <c r="E34" t="s">
+        <v>561</v>
+      </c>
+      <c r="F34" s="38" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="36"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="36"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
+      <c r="A35" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>552</v>
+      </c>
+      <c r="E35" t="s">
+        <v>558</v>
+      </c>
+      <c r="F35" s="38"/>
+    </row>
+    <row r="36" spans="1:6" ht="30.75">
+      <c r="A36" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>552</v>
+      </c>
+      <c r="E36" t="s">
+        <v>561</v>
+      </c>
+      <c r="F36" s="38" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="36"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="38"/>
+      <c r="A37" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>561</v>
+      </c>
+      <c r="E37" t="s">
+        <v>561</v>
+      </c>
+      <c r="F37" s="38" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="36"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="38"/>
+      <c r="A38" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>561</v>
+      </c>
+      <c r="E38" t="s">
+        <v>555</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="36"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="36"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
+      <c r="A39" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>581</v>
+      </c>
+      <c r="E39" t="s">
+        <v>553</v>
+      </c>
+      <c r="F39" s="38" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30.75">
+      <c r="A40" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>556</v>
+      </c>
+      <c r="E40" t="s">
+        <v>561</v>
+      </c>
+      <c r="F40" s="38" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="36"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>573</v>
+      </c>
+      <c r="E41" t="s">
+        <v>555</v>
+      </c>
       <c r="F41" s="38"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="36"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>555</v>
+      </c>
+      <c r="E42" t="s">
+        <v>553</v>
+      </c>
+      <c r="F42" s="38" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="36"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>552</v>
+      </c>
+      <c r="E43" t="s">
+        <v>555</v>
+      </c>
+      <c r="F43" s="38"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="36"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="38"/>
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>558</v>
+      </c>
+      <c r="E44" t="s">
+        <v>573</v>
+      </c>
+      <c r="F44" s="38" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="36"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>552</v>
+      </c>
+      <c r="E45" t="s">
+        <v>558</v>
+      </c>
       <c r="F45" s="38"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="36"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
+        <v>180</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>552</v>
+      </c>
+      <c r="E46" t="s">
+        <v>553</v>
+      </c>
+      <c r="F46" s="38" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="41"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>552</v>
+      </c>
+      <c r="E47" t="s">
+        <v>553</v>
+      </c>
+      <c r="F47" s="38" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="36"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>552</v>
+      </c>
+      <c r="E48" t="s">
+        <v>555</v>
+      </c>
+      <c r="F48" s="38"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="36"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>186</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>552</v>
+      </c>
+      <c r="E49" t="s">
+        <v>555</v>
+      </c>
+      <c r="F49" s="38"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="41"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>552</v>
+      </c>
+      <c r="E50" t="s">
+        <v>553</v>
+      </c>
+      <c r="F50" s="38" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="41"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>581</v>
+      </c>
+      <c r="E51" t="s">
+        <v>555</v>
+      </c>
+      <c r="F51" s="38" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="36"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>552</v>
+      </c>
+      <c r="E52" t="s">
+        <v>553</v>
+      </c>
+      <c r="F52" s="38" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="36"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>555</v>
+      </c>
+      <c r="E53" t="s">
+        <v>555</v>
+      </c>
       <c r="F53" s="38"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="36"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="36"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="s">
+        <v>468</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>552</v>
+      </c>
+      <c r="E54" t="s">
+        <v>555</v>
+      </c>
+      <c r="F54" s="38"/>
+    </row>
+    <row r="55" spans="1:6" ht="30.75">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>555</v>
+      </c>
+      <c r="E55" t="s">
+        <v>573</v>
+      </c>
+      <c r="F55" s="38" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="36"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
+      <c r="A56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>581</v>
+      </c>
+      <c r="E56" t="s">
+        <v>558</v>
+      </c>
+      <c r="F56" s="38" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="36"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>555</v>
+      </c>
+      <c r="E57" t="s">
+        <v>553</v>
+      </c>
+      <c r="F57" s="38" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="41"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="38"/>
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>552</v>
+      </c>
+      <c r="E58" t="s">
+        <v>558</v>
+      </c>
+      <c r="F58" s="38" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="41"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>191</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>552</v>
+      </c>
+      <c r="E59" t="s">
+        <v>555</v>
+      </c>
+      <c r="F59" s="38" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="36"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>555</v>
+      </c>
+      <c r="E60" t="s">
+        <v>555</v>
+      </c>
+      <c r="F60" s="38" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="41"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="38"/>
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>555</v>
+      </c>
+      <c r="E61" t="s">
+        <v>558</v>
+      </c>
+      <c r="F61" s="38" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="36"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="38"/>
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>194</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>561</v>
+      </c>
+      <c r="E62" t="s">
+        <v>558</v>
+      </c>
+      <c r="F62" s="38" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="36"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
+      <c r="A63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" t="s">
+        <v>195</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>552</v>
+      </c>
+      <c r="E63" t="s">
+        <v>555</v>
+      </c>
       <c r="F63" s="38"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="36"/>
-      <c r="B64" s="35"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="35"/>
+      <c r="A64" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>555</v>
+      </c>
+      <c r="E64" t="s">
+        <v>555</v>
+      </c>
+      <c r="F64" s="38" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="36"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="35"/>
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
+        <v>552</v>
+      </c>
+      <c r="E65" t="s">
+        <v>553</v>
+      </c>
+      <c r="F65" s="38" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="36"/>
-      <c r="B66" s="35"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="38"/>
+      <c r="A66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66">
+        <v>9</v>
+      </c>
+      <c r="D66" t="s">
+        <v>552</v>
+      </c>
+      <c r="E66" t="s">
+        <v>555</v>
+      </c>
+      <c r="F66" s="38" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="41"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" t="s">
+        <v>222</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>555</v>
+      </c>
+      <c r="E67" t="s">
+        <v>555</v>
+      </c>
+      <c r="F67" s="38"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="41"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="38"/>
+      <c r="A68" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" t="s">
+        <v>224</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>561</v>
+      </c>
+      <c r="E68" t="s">
+        <v>561</v>
+      </c>
+      <c r="F68" s="38" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="36"/>
-      <c r="B69" s="35"/>
-      <c r="C69" s="40"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" t="s">
+        <v>233</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>561</v>
+      </c>
+      <c r="E69" t="s">
+        <v>555</v>
+      </c>
+      <c r="F69" s="38" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="36"/>
-      <c r="B70" s="35"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="35"/>
+      <c r="A70" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" t="s">
+        <v>236</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>581</v>
+      </c>
+      <c r="E70" t="s">
+        <v>555</v>
+      </c>
+      <c r="F70" s="38" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="36"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="38"/>
+      <c r="A71" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" t="s">
+        <v>237</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>581</v>
+      </c>
+      <c r="E71" t="s">
+        <v>555</v>
+      </c>
+      <c r="F71" s="38" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="41"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
+      <c r="A72" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72" t="s">
+        <v>239</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>573</v>
+      </c>
+      <c r="E72" t="s">
+        <v>555</v>
+      </c>
+      <c r="F72" s="38"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="41"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="42"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
+      <c r="A73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" t="s">
+        <v>240</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>552</v>
+      </c>
+      <c r="E73" t="s">
+        <v>558</v>
+      </c>
+      <c r="F73" s="38" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="36"/>
-      <c r="B74" s="35"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="35"/>
+      <c r="A74" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" t="s">
+        <v>242</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>552</v>
+      </c>
+      <c r="E74" t="s">
+        <v>555</v>
+      </c>
+      <c r="F74" s="38"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="36"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
+      <c r="A75" t="s">
+        <v>35</v>
+      </c>
+      <c r="B75" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>555</v>
+      </c>
+      <c r="E75" t="s">
+        <v>555</v>
+      </c>
+      <c r="F75" s="38"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="41"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="38"/>
+      <c r="A76" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>561</v>
+      </c>
+      <c r="E76" t="s">
+        <v>558</v>
+      </c>
+      <c r="F76" s="38" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="36"/>
-      <c r="B77" s="35"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="35"/>
+      <c r="A77" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77" t="s">
+        <v>261</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>552</v>
+      </c>
+      <c r="E77" t="s">
+        <v>555</v>
+      </c>
+      <c r="F77" s="38"/>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="36"/>
-      <c r="B78" s="35"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="38"/>
+      <c r="A78" t="s">
+        <v>36</v>
+      </c>
+      <c r="B78" t="s">
+        <v>263</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>555</v>
+      </c>
+      <c r="E78" t="s">
+        <v>555</v>
+      </c>
+      <c r="F78" s="38" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="36"/>
-      <c r="B79" s="35"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
+      <c r="A79" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" t="s">
+        <v>264</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" t="s">
+        <v>552</v>
+      </c>
+      <c r="E79" t="s">
+        <v>555</v>
+      </c>
       <c r="F79" s="38"/>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="36"/>
-      <c r="B80" s="35"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="35"/>
+      <c r="A80" t="s">
+        <v>36</v>
+      </c>
+      <c r="B80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>555</v>
+      </c>
+      <c r="E80" t="s">
+        <v>558</v>
+      </c>
       <c r="F80" s="38"/>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="41"/>
-      <c r="B81" s="35"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="35"/>
-      <c r="E81" s="35"/>
-      <c r="F81" s="38"/>
+      <c r="A81" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81" t="s">
+        <v>76</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>552</v>
+      </c>
+      <c r="E81" t="s">
+        <v>561</v>
+      </c>
+      <c r="F81" s="38" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="36"/>
-      <c r="B82" s="35"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="35"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="38"/>
+      <c r="A82" t="s">
+        <v>36</v>
+      </c>
+      <c r="B82" t="s">
+        <v>266</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82" t="s">
+        <v>552</v>
+      </c>
+      <c r="E82" t="s">
+        <v>555</v>
+      </c>
+      <c r="F82" s="38" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="36"/>
-      <c r="B83" s="35"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="35"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="35"/>
+      <c r="A83" t="s">
+        <v>37</v>
+      </c>
+      <c r="B83" t="s">
+        <v>265</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>555</v>
+      </c>
+      <c r="E83" t="s">
+        <v>555</v>
+      </c>
+      <c r="F83" s="38" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="36"/>
-      <c r="B84" s="35"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="35"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="38"/>
+      <c r="A84" t="s">
+        <v>38</v>
+      </c>
+      <c r="B84" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>561</v>
+      </c>
+      <c r="F84" s="38" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="36"/>
-      <c r="B85" s="35"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="35"/>
-      <c r="E85" s="35"/>
-      <c r="F85" s="38"/>
+      <c r="A85" t="s">
+        <v>38</v>
+      </c>
+      <c r="B85" t="s">
+        <v>269</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>581</v>
+      </c>
+      <c r="E85" t="s">
+        <v>553</v>
+      </c>
+      <c r="F85" s="38" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="36"/>
-      <c r="B86" s="35"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="35"/>
+      <c r="A86" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" t="s">
+        <v>270</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>558</v>
+      </c>
+      <c r="E86" t="s">
+        <v>555</v>
+      </c>
+      <c r="F86" s="38"/>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="36"/>
-      <c r="B87" s="35"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="35"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="38"/>
+      <c r="A87" t="s">
+        <v>39</v>
+      </c>
+      <c r="B87" t="s">
+        <v>271</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>558</v>
+      </c>
+      <c r="E87" t="s">
+        <v>561</v>
+      </c>
+      <c r="F87" s="38" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="36"/>
-      <c r="B88" s="35"/>
-      <c r="C88" s="39"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="35"/>
+      <c r="A88" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
+        <v>552</v>
+      </c>
+      <c r="E88" t="s">
+        <v>555</v>
+      </c>
       <c r="F88" s="38"/>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="36"/>
-      <c r="B89" s="35"/>
-      <c r="C89" s="37"/>
-      <c r="D89" s="35"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="38"/>
+      <c r="A89" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="F89" s="38" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="36"/>
-      <c r="B90" s="35"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="35"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="35"/>
+      <c r="A90" t="s">
+        <v>39</v>
+      </c>
+      <c r="B90" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>555</v>
+      </c>
+      <c r="E90" t="s">
+        <v>558</v>
+      </c>
+      <c r="F90" s="38" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="36"/>
-      <c r="B91" s="35"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="35"/>
-      <c r="E91" s="35"/>
-      <c r="F91" s="35"/>
+      <c r="A91" t="s">
+        <v>39</v>
+      </c>
+      <c r="B91" t="s">
+        <v>272</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>552</v>
+      </c>
+      <c r="E91" t="s">
+        <v>553</v>
+      </c>
+      <c r="F91" s="38" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="36"/>
-      <c r="B92" s="35"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="35"/>
-      <c r="E92" s="35"/>
-      <c r="F92" s="38"/>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" s="36"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="39"/>
-      <c r="D93" s="35"/>
-      <c r="E93" s="35"/>
-      <c r="F93" s="38"/>
+      <c r="A92" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" t="s">
+        <v>273</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>561</v>
+      </c>
+      <c r="E92" t="s">
+        <v>573</v>
+      </c>
+      <c r="F92" s="38" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="30.75">
+      <c r="A93" t="s">
+        <v>41</v>
+      </c>
+      <c r="B93" t="s">
+        <v>166</v>
+      </c>
+      <c r="C93">
+        <v>4</v>
+      </c>
+      <c r="D93" t="s">
+        <v>561</v>
+      </c>
+      <c r="E93" t="s">
+        <v>561</v>
+      </c>
+      <c r="F93" s="38" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="36"/>
-      <c r="B94" s="35"/>
-      <c r="C94" s="37"/>
-      <c r="D94" s="35"/>
-      <c r="E94" s="35"/>
-      <c r="F94" s="35"/>
+      <c r="A94" t="s">
+        <v>41</v>
+      </c>
+      <c r="B94" t="s">
+        <v>274</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94" t="s">
+        <v>561</v>
+      </c>
+      <c r="E94" t="s">
+        <v>561</v>
+      </c>
+      <c r="F94" s="38" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="36"/>
-      <c r="B95" s="35"/>
-      <c r="C95" s="42"/>
-      <c r="D95" s="35"/>
-      <c r="E95" s="35"/>
-      <c r="F95" s="35"/>
+      <c r="A95" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" t="s">
+        <v>69</v>
+      </c>
+      <c r="C95">
+        <v>5</v>
+      </c>
+      <c r="D95" t="s">
+        <v>558</v>
+      </c>
+      <c r="E95" t="s">
+        <v>555</v>
+      </c>
+      <c r="F95" s="38"/>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="36"/>
-      <c r="B96" s="35"/>
-      <c r="C96" s="46"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="35"/>
-      <c r="F96" s="35"/>
+      <c r="A96" t="s">
+        <v>43</v>
+      </c>
+      <c r="B96" t="s">
+        <v>278</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>561</v>
+      </c>
+      <c r="E96" t="s">
+        <v>558</v>
+      </c>
+      <c r="F96" s="38" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="36"/>
-      <c r="B97" s="35"/>
-      <c r="C97" s="43"/>
-      <c r="D97" s="35"/>
-      <c r="E97" s="35"/>
-      <c r="F97" s="35"/>
+      <c r="A97" t="s">
+        <v>43</v>
+      </c>
+      <c r="B97" t="s">
+        <v>279</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>555</v>
+      </c>
+      <c r="E97" t="s">
+        <v>555</v>
+      </c>
+      <c r="F97" s="38"/>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="36"/>
-      <c r="B98" s="35"/>
-      <c r="C98" s="43"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="35"/>
+      <c r="A98" t="s">
+        <v>44</v>
+      </c>
+      <c r="B98" t="s">
+        <v>144</v>
+      </c>
+      <c r="C98">
+        <v>3</v>
+      </c>
+      <c r="D98" t="s">
+        <v>552</v>
+      </c>
+      <c r="E98" t="s">
+        <v>555</v>
+      </c>
+      <c r="F98" s="38"/>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="41"/>
-      <c r="B99" s="35"/>
-      <c r="C99" s="42"/>
-      <c r="D99" s="35"/>
-      <c r="E99" s="35"/>
-      <c r="F99" s="35"/>
+      <c r="A99" t="s">
+        <v>44</v>
+      </c>
+      <c r="B99" t="s">
+        <v>71</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>561</v>
+      </c>
+      <c r="E99" t="s">
+        <v>558</v>
+      </c>
+      <c r="F99" s="38" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="41"/>
-      <c r="B100" s="35"/>
-      <c r="C100" s="39"/>
-      <c r="D100" s="35"/>
-      <c r="E100" s="35"/>
-      <c r="F100" s="38"/>
+      <c r="A100" t="s">
+        <v>46</v>
+      </c>
+      <c r="B100" t="s">
+        <v>290</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>555</v>
+      </c>
+      <c r="E100" t="s">
+        <v>558</v>
+      </c>
+      <c r="F100" s="38" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="36"/>
-      <c r="B101" s="35"/>
-      <c r="C101" s="37"/>
-      <c r="D101" s="35"/>
-      <c r="E101" s="35"/>
+      <c r="A101" t="s">
+        <v>46</v>
+      </c>
+      <c r="B101" t="s">
+        <v>340</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>552</v>
+      </c>
+      <c r="E101" t="s">
+        <v>573</v>
+      </c>
       <c r="F101" s="38"/>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="36"/>
-      <c r="B102" s="35"/>
-      <c r="C102" s="37"/>
-      <c r="D102" s="35"/>
-      <c r="E102" s="35"/>
-      <c r="F102" s="35"/>
+      <c r="A102" t="s">
+        <v>46</v>
+      </c>
+      <c r="B102" t="s">
+        <v>298</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102" t="s">
+        <v>561</v>
+      </c>
+      <c r="E102" t="s">
+        <v>558</v>
+      </c>
+      <c r="F102" s="38" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="36"/>
-      <c r="B103" s="35"/>
-      <c r="C103" s="37"/>
-      <c r="D103" s="35"/>
-      <c r="E103" s="35"/>
+      <c r="A103" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103" t="s">
+        <v>303</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103" t="s">
+        <v>552</v>
+      </c>
+      <c r="E103" t="s">
+        <v>555</v>
+      </c>
       <c r="F103" s="38"/>
     </row>
-    <row r="104" spans="1:6">
-      <c r="A104" s="36"/>
-      <c r="B104" s="35"/>
-      <c r="C104" s="37"/>
-      <c r="D104" s="35"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="38"/>
+    <row r="104" spans="1:6" ht="30.75">
+      <c r="A104" t="s">
+        <v>46</v>
+      </c>
+      <c r="B104" t="s">
+        <v>339</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
+      </c>
+      <c r="D104" t="s">
+        <v>556</v>
+      </c>
+      <c r="E104" t="s">
+        <v>561</v>
+      </c>
+      <c r="F104" s="38" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="36"/>
-      <c r="B105" s="35"/>
-      <c r="C105" s="37"/>
-      <c r="D105" s="35"/>
-      <c r="E105" s="35"/>
-      <c r="F105" s="38"/>
+      <c r="A105" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105" t="s">
+        <v>315</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>556</v>
+      </c>
+      <c r="E105" t="s">
+        <v>555</v>
+      </c>
+      <c r="F105" s="38" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="36"/>
-      <c r="B106" s="35"/>
-      <c r="C106" s="37"/>
-      <c r="D106" s="35"/>
-      <c r="E106" s="35"/>
+      <c r="A106" t="s">
+        <v>46</v>
+      </c>
+      <c r="B106" t="s">
+        <v>321</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="D106" t="s">
+        <v>552</v>
+      </c>
+      <c r="E106" t="s">
+        <v>555</v>
+      </c>
       <c r="F106" s="38"/>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="36"/>
-      <c r="B107" s="35"/>
-      <c r="C107" s="37"/>
-      <c r="D107" s="35"/>
-      <c r="E107" s="35"/>
-      <c r="F107" s="38"/>
+      <c r="A107" t="s">
+        <v>46</v>
+      </c>
+      <c r="B107" t="s">
+        <v>327</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107" t="s">
+        <v>552</v>
+      </c>
+      <c r="E107" t="s">
+        <v>553</v>
+      </c>
+      <c r="F107" s="38" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="41"/>
-      <c r="B108" s="35"/>
-      <c r="C108" s="37"/>
-      <c r="D108" s="35"/>
-      <c r="E108" s="35"/>
+      <c r="A108" t="s">
+        <v>46</v>
+      </c>
+      <c r="B108" t="s">
+        <v>331</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
+      </c>
+      <c r="D108" t="s">
+        <v>552</v>
+      </c>
+      <c r="E108" t="s">
+        <v>555</v>
+      </c>
       <c r="F108" s="38"/>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="41"/>
-      <c r="B109" s="35"/>
-      <c r="C109" s="40"/>
-      <c r="D109" s="35"/>
-      <c r="E109" s="35"/>
-      <c r="F109" s="38"/>
+      <c r="A109" t="s">
+        <v>46</v>
+      </c>
+      <c r="B109" t="s">
+        <v>332</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>552</v>
+      </c>
+      <c r="E109" t="s">
+        <v>561</v>
+      </c>
+      <c r="F109" s="38" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" t="s">
+        <v>46</v>
+      </c>
+      <c r="B110" t="s">
+        <v>333</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>558</v>
+      </c>
+      <c r="E110" t="s">
+        <v>555</v>
+      </c>
+      <c r="F110" s="38"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>46</v>
+      </c>
+      <c r="B111" t="s">
+        <v>151</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" t="s">
+        <v>552</v>
+      </c>
+      <c r="E111" t="s">
+        <v>573</v>
+      </c>
+      <c r="F111" s="38"/>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" t="s">
+        <v>49</v>
+      </c>
+      <c r="B112" t="s">
+        <v>374</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" t="s">
+        <v>552</v>
+      </c>
+      <c r="E112" t="s">
+        <v>555</v>
+      </c>
+      <c r="F112" s="38"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" t="s">
+        <v>51</v>
+      </c>
+      <c r="B113" t="s">
+        <v>95</v>
+      </c>
+      <c r="C113">
+        <v>4</v>
+      </c>
+      <c r="D113" t="s">
+        <v>555</v>
+      </c>
+      <c r="E113" t="s">
+        <v>561</v>
+      </c>
+      <c r="F113" s="38" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" t="s">
+        <v>51</v>
+      </c>
+      <c r="B114" t="s">
+        <v>401</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
+        <v>555</v>
+      </c>
+      <c r="E114" t="s">
+        <v>555</v>
+      </c>
+      <c r="F114" s="38"/>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" t="s">
+        <v>51</v>
+      </c>
+      <c r="B115" t="s">
+        <v>402</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+      <c r="D115" t="s">
+        <v>573</v>
+      </c>
+      <c r="E115" t="s">
+        <v>561</v>
+      </c>
+      <c r="F115" s="38" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" t="s">
+        <v>51</v>
+      </c>
+      <c r="B116" t="s">
+        <v>403</v>
+      </c>
+      <c r="C116">
+        <v>4</v>
+      </c>
+      <c r="D116" t="s">
+        <v>552</v>
+      </c>
+      <c r="E116" t="s">
+        <v>555</v>
+      </c>
+      <c r="F116" s="38" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" t="s">
+        <v>51</v>
+      </c>
+      <c r="B117" t="s">
+        <v>412</v>
+      </c>
+      <c r="C117">
+        <v>5</v>
+      </c>
+      <c r="D117" t="s">
+        <v>552</v>
+      </c>
+      <c r="E117" t="s">
+        <v>558</v>
+      </c>
+      <c r="F117" s="38"/>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" t="s">
+        <v>52</v>
+      </c>
+      <c r="B118" t="s">
+        <v>144</v>
+      </c>
+      <c r="C118">
+        <v>9</v>
+      </c>
+      <c r="D118" t="s">
+        <v>552</v>
+      </c>
+      <c r="E118" t="s">
+        <v>561</v>
+      </c>
+      <c r="F118" s="38" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="30.75">
+      <c r="A119" t="s">
+        <v>52</v>
+      </c>
+      <c r="B119" t="s">
+        <v>165</v>
+      </c>
+      <c r="C119">
+        <v>4</v>
+      </c>
+      <c r="D119" t="s">
+        <v>581</v>
+      </c>
+      <c r="E119" t="s">
+        <v>561</v>
+      </c>
+      <c r="F119" s="38" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="30.75">
+      <c r="A120" t="s">
+        <v>52</v>
+      </c>
+      <c r="B120" t="s">
+        <v>425</v>
+      </c>
+      <c r="C120">
+        <v>5</v>
+      </c>
+      <c r="D120" t="s">
+        <v>573</v>
+      </c>
+      <c r="E120" t="s">
+        <v>555</v>
+      </c>
+      <c r="F120" s="38" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" t="s">
+        <v>52</v>
+      </c>
+      <c r="B121" t="s">
+        <v>147</v>
+      </c>
+      <c r="C121">
+        <v>6</v>
+      </c>
+      <c r="D121" t="s">
+        <v>555</v>
+      </c>
+      <c r="E121" t="s">
+        <v>558</v>
+      </c>
+      <c r="F121" s="38" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" t="s">
+        <v>53</v>
+      </c>
+      <c r="B122" t="s">
+        <v>426</v>
+      </c>
+      <c r="C122">
+        <v>7</v>
+      </c>
+      <c r="D122" t="s">
+        <v>552</v>
+      </c>
+      <c r="E122" t="s">
+        <v>558</v>
+      </c>
+      <c r="F122" s="38" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" t="s">
+        <v>54</v>
+      </c>
+      <c r="B123" t="s">
+        <v>440</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123" t="s">
+        <v>552</v>
+      </c>
+      <c r="E123" t="s">
+        <v>561</v>
+      </c>
+      <c r="F123" s="38" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" t="s">
+        <v>54</v>
+      </c>
+      <c r="B124" t="s">
+        <v>467</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124" t="s">
+        <v>552</v>
+      </c>
+      <c r="E124" t="s">
+        <v>561</v>
+      </c>
+      <c r="F124" s="38" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" t="s">
+        <v>54</v>
+      </c>
+      <c r="B125" t="s">
+        <v>462</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="D125" t="s">
+        <v>555</v>
+      </c>
+      <c r="E125" t="s">
+        <v>555</v>
+      </c>
+      <c r="F125" s="38"/>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" t="s">
+        <v>54</v>
+      </c>
+      <c r="B126" t="s">
+        <v>436</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126" t="s">
+        <v>555</v>
+      </c>
+      <c r="E126" t="s">
+        <v>555</v>
+      </c>
+      <c r="F126" s="38"/>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" t="s">
+        <v>54</v>
+      </c>
+      <c r="B127" t="s">
+        <v>451</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127" t="s">
+        <v>552</v>
+      </c>
+      <c r="E127" t="s">
+        <v>561</v>
+      </c>
+      <c r="F127" s="38" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" t="s">
+        <v>54</v>
+      </c>
+      <c r="B128" t="s">
+        <v>463</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128" t="s">
+        <v>561</v>
+      </c>
+      <c r="E128" t="s">
+        <v>561</v>
+      </c>
+      <c r="F128" s="38" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" t="s">
+        <v>54</v>
+      </c>
+      <c r="B129" t="s">
+        <v>447</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129" t="s">
+        <v>552</v>
+      </c>
+      <c r="E129" t="s">
+        <v>555</v>
+      </c>
+      <c r="F129" s="38"/>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" t="s">
+        <v>54</v>
+      </c>
+      <c r="B130" t="s">
+        <v>437</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130" t="s">
+        <v>555</v>
+      </c>
+      <c r="E130" t="s">
+        <v>561</v>
+      </c>
+      <c r="F130" s="38" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" t="s">
+        <v>54</v>
+      </c>
+      <c r="B131" t="s">
+        <v>446</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131" t="s">
+        <v>555</v>
+      </c>
+      <c r="E131" t="s">
+        <v>555</v>
+      </c>
+      <c r="F131" s="38"/>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>54</v>
+      </c>
+      <c r="B132" t="s">
+        <v>460</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+      <c r="D132" t="s">
+        <v>558</v>
+      </c>
+      <c r="E132" t="s">
+        <v>573</v>
+      </c>
+      <c r="F132" s="38" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>54</v>
+      </c>
+      <c r="B133" t="s">
+        <v>107</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133" t="s">
+        <v>561</v>
+      </c>
+      <c r="E133" t="s">
+        <v>561</v>
+      </c>
+      <c r="F133" s="38" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="s">
+        <v>54</v>
+      </c>
+      <c r="B134" t="s">
+        <v>429</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134" t="s">
+        <v>552</v>
+      </c>
+      <c r="E134" t="s">
+        <v>561</v>
+      </c>
+      <c r="F134" s="38" t="s">
+        <v>636</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C39">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C134">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>